<commit_message>
Update hot topic list Jan 2019.xlsx
</commit_message>
<xml_diff>
--- a/hot topic list Jan 2019.xlsx
+++ b/hot topic list Jan 2019.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Conferences and papers\CTN\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="14460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Hot topic name</t>
   </si>
@@ -39,6 +37,18 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>THz frequencies: communication meets positioning</t>
+  </si>
+  <si>
+    <t>Angel?</t>
+  </si>
+  <si>
+    <t>The next frontier after mmWave seems to be THz frequencies, where signals can simultaneously serve to communicate (short range) and to position with high resolution</t>
+  </si>
+  <si>
+    <t>blockchain for comms</t>
   </si>
 </sst>
 </file>
@@ -144,7 +154,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,7 +189,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -356,7 +366,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -364,20 +374,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="196" zoomScaleNormal="196" zoomScalePageLayoutView="196" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="48.85546875" customWidth="1"/>
+    <col min="1" max="1" width="40.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="48.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -388,16 +398,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>